<commit_message>
Storyboard revisions for Build a WP
</commit_message>
<xml_diff>
--- a/assets/fr/Budget_annee_derniere.xlsx
+++ b/assets/fr/Budget_annee_derniere.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csabouri\Documents\GitHub\adt_finance_prototype\assets\fr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BLord\github\adt_finance-R1\assets\fr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD87684-F0A1-4AAF-8615-869C71C279E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Template FR" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <customWorkbookViews>
     <customWorkbookView name="Filter 1" guid="{EA7869F4-D147-4A50-842C-3DF5486AE805}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
@@ -36,13 +35,6 @@
     <t>Poste individuel</t>
   </si>
   <si>
-    <t>Budget Précédent</t>
-  </si>
-  <si>
-    <t>Budget 
-Actuel</t>
-  </si>
-  <si>
     <t>Budget proposé</t>
   </si>
   <si>
@@ -91,19 +83,25 @@
     <t>Voyage</t>
   </si>
   <si>
-    <t>10 000 $ pour effectuer des inspections, 1,6 000 $ pour les déplacements généraux</t>
-  </si>
-  <si>
     <t>Aide temporaire</t>
   </si>
   <si>
     <t>pour aider à effectuer des inspections à distance</t>
+  </si>
+  <si>
+    <t>Précédent</t>
+  </si>
+  <si>
+    <t>Actuel</t>
+  </si>
+  <si>
+    <t>10 000 $ pour effectuer des inspections, 16 000 $ pour les déplacements généraux</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="#\ ##0\ [$$]"/>
@@ -459,61 +457,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
-    <col min="7" max="7" width="61.5546875" customWidth="1"/>
+    <col min="2" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="26"/>
       <c r="F1" s="26"/>
       <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -522,9 +522,9 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="9">
         <v>460000</v>
@@ -543,12 +543,12 @@
         <v>443333</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="15">
         <f t="shared" ref="B7:E7" si="1">SUM(B6)</f>
@@ -571,16 +571,16 @@
         <v>443333</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -589,16 +589,16 @@
       <c r="F9" s="17"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="19">
         <v>0</v>
@@ -615,12 +615,12 @@
         <v>3000</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="19">
         <v>1961</v>
@@ -637,12 +637,12 @@
         <v>1500</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="19">
         <v>2000</v>
@@ -661,12 +661,12 @@
         <v>4400</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" s="19">
         <v>18000</v>
@@ -685,12 +685,12 @@
         <v>11600</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15" s="22">
         <v>10000</v>
@@ -709,12 +709,12 @@
         <v>6000</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" s="15">
         <f t="shared" ref="B16:E16" si="3">SUM(B11:B15)</f>

</xml_diff>